<commit_message>
Add small modification to sheet
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Test 1</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Memory (kb)</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Mac : 2.4 i7 4 GB DDR</t>
+  </si>
+  <si>
+    <t>Web</t>
   </si>
 </sst>
 </file>
@@ -91,8 +100,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -107,17 +118,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -459,236 +472,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="B2" t="s">
+    <row r="3" spans="1:11">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>1.869</v>
-      </c>
-      <c r="C3">
-        <v>83</v>
-      </c>
-      <c r="D3">
-        <v>1.901</v>
-      </c>
-      <c r="E3">
-        <v>82.1</v>
-      </c>
-      <c r="F3">
-        <v>2.0550000000000002</v>
-      </c>
-      <c r="G3">
-        <v>83.5</v>
-      </c>
-      <c r="H3">
-        <v>2.7639999999999998</v>
-      </c>
-      <c r="I3">
-        <v>86.6</v>
-      </c>
-      <c r="J3">
-        <v>1.9319999999999999</v>
-      </c>
-      <c r="K3">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="B4">
-        <v>3.4820000000000002</v>
+        <v>1.869</v>
       </c>
       <c r="C4">
-        <v>186</v>
+        <v>83</v>
       </c>
       <c r="D4">
-        <v>3.18</v>
+        <v>1.901</v>
       </c>
       <c r="E4">
-        <v>191</v>
+        <v>82.1</v>
       </c>
       <c r="F4">
-        <v>4.2859999999999996</v>
+        <v>2.0550000000000002</v>
       </c>
       <c r="G4">
-        <v>189</v>
+        <v>83.5</v>
       </c>
       <c r="H4">
-        <v>2.9689999999999999</v>
+        <v>2.7639999999999998</v>
       </c>
       <c r="I4">
-        <v>188</v>
+        <v>86.6</v>
       </c>
       <c r="J4">
-        <v>3.4870000000000001</v>
+        <v>1.9319999999999999</v>
       </c>
       <c r="K4">
-        <v>190</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="B5">
-        <v>6.1470000000000002</v>
+        <v>3.4820000000000002</v>
       </c>
       <c r="C5">
-        <v>370</v>
+        <v>186</v>
       </c>
       <c r="D5">
-        <v>5.9409999999999998</v>
+        <v>3.18</v>
       </c>
       <c r="E5">
-        <v>371</v>
+        <v>191</v>
       </c>
       <c r="F5">
-        <v>6.0839999999999996</v>
+        <v>4.2859999999999996</v>
       </c>
       <c r="G5">
-        <v>369</v>
+        <v>189</v>
       </c>
       <c r="H5">
-        <v>7.2569999999999997</v>
+        <v>2.9689999999999999</v>
       </c>
       <c r="I5">
-        <v>371</v>
+        <v>188</v>
       </c>
       <c r="J5">
-        <v>6.056</v>
+        <v>3.4870000000000001</v>
       </c>
       <c r="K5">
-        <v>368</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B6">
-        <v>11.064</v>
+        <v>6.1470000000000002</v>
       </c>
       <c r="C6">
-        <v>721</v>
+        <v>370</v>
       </c>
       <c r="D6">
-        <v>9.4589999999999996</v>
+        <v>5.9409999999999998</v>
       </c>
       <c r="E6">
-        <v>729</v>
+        <v>371</v>
       </c>
       <c r="F6">
-        <v>11.013999999999999</v>
+        <v>6.0839999999999996</v>
       </c>
       <c r="G6">
-        <v>724</v>
+        <v>369</v>
       </c>
       <c r="H6">
-        <v>10.412000000000001</v>
+        <v>7.2569999999999997</v>
       </c>
       <c r="I6">
-        <v>723</v>
+        <v>371</v>
       </c>
       <c r="J6">
-        <v>10.83</v>
+        <v>6.056</v>
       </c>
       <c r="K6">
-        <v>724</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="B7">
-        <v>19.550999999999998</v>
+        <v>11.064</v>
       </c>
       <c r="C7">
-        <v>1800</v>
+        <v>721</v>
       </c>
       <c r="D7">
-        <v>18.555</v>
+        <v>9.4589999999999996</v>
       </c>
       <c r="E7">
-        <v>1700</v>
+        <v>729</v>
       </c>
       <c r="F7">
-        <v>20.212</v>
+        <v>11.013999999999999</v>
       </c>
       <c r="G7">
-        <v>1900</v>
+        <v>724</v>
       </c>
       <c r="H7">
-        <v>19.100000000000001</v>
+        <v>10.412000000000001</v>
       </c>
       <c r="I7">
-        <v>1850</v>
+        <v>723</v>
       </c>
       <c r="J7">
-        <v>19.111999999999998</v>
+        <v>10.83</v>
       </c>
       <c r="K7">
-        <v>1900</v>
+        <v>724</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>10000</v>
+        <v>2500</v>
+      </c>
+      <c r="B8">
+        <v>19.550999999999998</v>
+      </c>
+      <c r="C8">
+        <v>1800</v>
+      </c>
+      <c r="D8">
+        <v>18.555</v>
+      </c>
+      <c r="E8">
+        <v>1700</v>
+      </c>
+      <c r="F8">
+        <v>20.212</v>
+      </c>
+      <c r="G8">
+        <v>1900</v>
+      </c>
+      <c r="H8">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="I8">
+        <v>1850</v>
+      </c>
+      <c r="J8">
+        <v>19.111999999999998</v>
+      </c>
+      <c r="K8">
+        <v>1900</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
         <v>21000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding view of 20 point for testing purpuse on different devices
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Test 1</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Web</t>
+  </si>
+  <si>
+    <t>Avarage</t>
   </si>
 </sst>
 </file>
@@ -100,8 +103,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -118,19 +123,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="M4" sqref="M4:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -471,7 +478,7 @@
     <col min="1" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -482,7 +489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -498,8 +505,11 @@
       <c r="K2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -531,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>100</v>
       </c>
@@ -565,8 +575,16 @@
       <c r="K4">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <f>AVERAGE(B4,D4,F4,H4,J4)</f>
+        <v>2.1042000000000001</v>
+      </c>
+      <c r="M4">
+        <f>AVERAGE(C4,E4,G4,I4,K4)</f>
+        <v>83.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>250</v>
       </c>
@@ -600,8 +618,16 @@
       <c r="K5">
         <v>190</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <f t="shared" ref="L5:L8" si="0">AVERAGE(B5,D5,F5,H5,J5)</f>
+        <v>3.4807999999999999</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M8" si="1">AVERAGE(C5,E5,G5,I5,K5)</f>
+        <v>188.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>500</v>
       </c>
@@ -635,8 +661,16 @@
       <c r="K6">
         <v>368</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>6.2970000000000006</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>369.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -670,8 +704,16 @@
       <c r="K7">
         <v>724</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>10.5558</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>724.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>2500</v>
       </c>
@@ -705,13 +747,21 @@
       <c r="K8">
         <v>1900</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>19.306000000000001</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>21000</v>
       </c>

</xml_diff>